<commit_message>
Transfer the master to abbi branch
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdkil\eclipse-workspace\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OmarHiba\git\FrameworkFromScratch\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC50C6EC-AD7F-4EDB-9853-62B14047BE1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AB8C34-5BF3-4A49-9AB6-B6455F88479E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D002B59F-1738-4FB9-9DED-9569BFBC4008}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8994" xr2:uid="{D002B59F-1738-4FB9-9DED-9569BFBC4008}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -418,12 +418,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -451,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -465,7 +465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>

</xml_diff>